<commit_message>
feat: aactualizo roadmap con TC-02: Loguin Fallido
</commit_message>
<xml_diff>
--- a/docs/QA_Roadmap_Natalia.xlsx
+++ b/docs/QA_Roadmap_Natalia.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Hoja 2" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Actualización de Test Case Auto" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -19,37 +19,116 @@
     <t>Título del Test</t>
   </si>
   <si>
-    <t>Precondición</t>
-  </si>
-  <si>
-    <t>Pasos (Micro-pasos)</t>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Selector</t>
+  </si>
+  <si>
+    <t>Automatizado</t>
+  </si>
+  <si>
+    <t>Resultado Final</t>
+  </si>
+  <si>
+    <t>Fecha de Ejecución</t>
+  </si>
+  <si>
+    <t>Paso</t>
+  </si>
+  <si>
+    <t>Acción Técnica (Comentario en Código)</t>
   </si>
   <si>
     <t>Resultado Esperado</t>
   </si>
   <si>
-    <t>TC-03</t>
-  </si>
-  <si>
-    <t>Validación de Formato de Email</t>
-  </si>
-  <si>
-    <t>Estar en la pantalla de Login.</t>
-  </si>
-  <si>
-    <t>1. Ingresar texto sin "@" (ej: "natalia-test"). 
-2. Ingresar password. 
-3. Click en "Enviar".</t>
-  </si>
-  <si>
-    <t>El sistema muestra error de "Formato de email no válido" y no procesa el envío.</t>
+    <t>TC-01</t>
+  </si>
+  <si>
+    <t>Login Exitoso (Happy Path)</t>
+  </si>
+  <si>
+    <t>P0 (Crítica)</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>#login-button, [data-test="username"]</t>
+  </si>
+  <si>
+    <t>✅ SÍ (Playwright)</t>
+  </si>
+  <si>
+    <t>PASSED 🟢</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Navegar a la página</t>
+  </si>
+  <si>
+    <t>La página carga correctamente.</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>Ingresar credenciales</t>
+  </si>
+  <si>
+    <t>Los campos de texto aceptan la entrada.</t>
+  </si>
+  <si>
+    <t>Click en el botón de login</t>
+  </si>
+  <si>
+    <t>Se procesa la solicitud de acceso.</t>
+  </si>
+  <si>
+    <t>Validar que entramos (Aserción)</t>
+  </si>
+  <si>
+    <t>La URL es https://www.saucedemo.com/inventory.html.</t>
+  </si>
+  <si>
+    <t>TC-02</t>
+  </si>
+  <si>
+    <t>Loguin Fallido (Pasword incorrecto)</t>
+  </si>
+  <si>
+    <t>[data-test="login-button"], [data-test="username"], [data-test="password"]</t>
+  </si>
+  <si>
+    <t>Ir a la página.</t>
+  </si>
+  <si>
+    <t>Escribir usuario válido.</t>
+  </si>
+  <si>
+    <t>El campo de texto acepta la entrada.</t>
+  </si>
+  <si>
+    <t>Escribir password inválido.</t>
+  </si>
+  <si>
+    <t>Click en Login.</t>
+  </si>
+  <si>
+    <t>La URL se mantiene igual y aparece el mensaje de error: 'Epic sadface: Password is required' (o el que corresponda).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -61,13 +140,23 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -76,92 +165,39 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF535FC1"/>
-          <bgColor rgb="FF535FC1"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF535FC1"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF535FC1"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF535FC1"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF535FC1"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1">
-    <tableStyle count="4" pivot="0" name="Hoja 2-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
@@ -169,17 +205,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E2" displayName="Tabla_1" name="Tabla_1" id="1">
-  <tableColumns count="5">
-    <tableColumn name="ID" id="1"/>
-    <tableColumn name="Título del Test" id="2"/>
-    <tableColumn name="Precondición" id="3"/>
-    <tableColumn name="Pasos (Micro-pasos)" id="4"/>
-    <tableColumn name="Resultado Esperado" id="5"/>
-  </tableColumns>
-  <tableStyleInfo name="Hoja 2-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,21 +409,23 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.0"/>
-    <col customWidth="1" min="2" max="2" width="25.63"/>
-    <col customWidth="1" min="3" max="3" width="23.5"/>
-    <col customWidth="1" min="4" max="4" width="33.25"/>
-    <col customWidth="1" min="5" max="5" width="36.5"/>
+    <col customWidth="1" min="1" max="1" width="5.63"/>
+    <col customWidth="1" min="2" max="2" width="21.25"/>
+    <col customWidth="1" min="3" max="3" width="9.38"/>
+    <col customWidth="1" min="4" max="4" width="8.63"/>
+    <col customWidth="1" min="5" max="6" width="14.38"/>
+    <col customWidth="1" min="7" max="7" width="12.63"/>
+    <col customWidth="1" min="8" max="8" width="15.63"/>
+    <col customWidth="1" min="9" max="9" width="4.75"/>
+    <col customWidth="1" min="10" max="10" width="30.5"/>
+    <col customWidth="1" min="11" max="11" width="41.75"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22.5" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,34 +435,465 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5">
+        <v>46035.0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="5">
+        <v>46036.0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: Update QA roadmap with TC-04 test
</commit_message>
<xml_diff>
--- a/docs/QA_Roadmap_Natalia.xlsx
+++ b/docs/QA_Roadmap_Natalia.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -140,6 +140,27 @@
   </si>
   <si>
     <t>Username is required</t>
+  </si>
+  <si>
+    <t>TC-04</t>
+  </si>
+  <si>
+    <t>Validar carga de productos (Happy Path)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iniciar sesion con credenciales validas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validar que entramos a pagina Productos</t>
+  </si>
+  <si>
+    <t>El titulo de la pagina es Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validar que se cargan los productos correctamente.</t>
+  </si>
+  <si>
+    <t>Se encuentran 6 productos</t>
   </si>
 </sst>
 </file>
@@ -186,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -215,6 +236,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -977,6 +1001,86 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="10">
+        <v>46053.0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="I16" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="I17" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="I18" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: update readme content, qa roadmap TC-05 test and gitignore
</commit_message>
<xml_diff>
--- a/docs/QA_Roadmap_Natalia.xlsx
+++ b/docs/QA_Roadmap_Natalia.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -148,6 +148,9 @@
     <t>Validar carga de productos (Happy Path)</t>
   </si>
   <si>
+    <t>[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title, .inventory_item_price</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Iniciar sesion con credenciales validas</t>
   </si>
   <si>
@@ -161,6 +164,44 @@
   </si>
   <si>
     <t>Se encuentran 6 productos</t>
+  </si>
+  <si>
+    <t>TC-05</t>
+  </si>
+  <si>
+    <t>Validar el formato de precios ($)</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>.inventory_item_price</t>
+    </r>
+  </si>
+  <si>
+    <t>Validar carga de la página de inventario.</t>
+  </si>
+  <si>
+    <t>El título de la página es "Products" y el contenedor de ítems es visible.</t>
+  </si>
+  <si>
+    <t>Extraer lista de precios y verificar el símbolo de moneda.</t>
+  </si>
+  <si>
+    <t>Todos los precios contienen el símbolo "$" y el formato es numérico válido.</t>
   </si>
 </sst>
 </file>
@@ -170,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -185,6 +226,12 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -207,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -219,6 +266,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
@@ -233,13 +283,16 @@
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,7 +510,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -465,7 +521,7 @@
     <col customWidth="1" min="2" max="2" width="20.75"/>
     <col customWidth="1" min="3" max="3" width="9.38"/>
     <col customWidth="1" min="4" max="4" width="8.63"/>
-    <col customWidth="1" min="5" max="5" width="20.75"/>
+    <col customWidth="1" min="5" max="5" width="33.63"/>
     <col customWidth="1" min="6" max="6" width="14.38"/>
     <col customWidth="1" min="7" max="7" width="12.63"/>
     <col customWidth="1" min="8" max="8" width="11.13"/>
@@ -539,22 +595,22 @@
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="6">
         <v>46035.0</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="7">
         <v>1.0</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -584,14 +640,14 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="6">
+      <c r="I3" s="7">
         <v>2.0</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -621,14 +677,14 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="6">
+      <c r="I4" s="7">
         <v>3.0</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -658,14 +714,14 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="6">
+      <c r="I5" s="7">
         <v>4.0</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -695,11 +751,11 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="1"/>
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
@@ -732,19 +788,19 @@
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="6">
         <v>46036.0</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="7">
         <v>1.0</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -777,17 +833,16 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="6">
+      <c r="I8" s="7">
         <v>2.0</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -814,17 +869,16 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="6">
+      <c r="I9" s="7">
         <v>3.0</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -851,17 +905,16 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="6">
+      <c r="I10" s="7">
         <v>4.0</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -896,22 +949,22 @@
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="6">
         <v>46048.0</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="7">
         <v>1.0</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="10" t="s">
         <v>38</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -941,17 +994,16 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="6">
+      <c r="I12" s="7">
         <v>2.0</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -974,13 +1026,13 @@
       <c r="AA12" s="3"/>
     </row>
     <row r="13">
-      <c r="I13" s="6">
+      <c r="I13" s="7">
         <v>3.0</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -988,13 +1040,13 @@
       </c>
     </row>
     <row r="14">
-      <c r="I14" s="6">
+      <c r="I14" s="7">
         <v>4.0</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="10" t="s">
         <v>42</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1002,10 +1054,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1014,22 +1066,22 @@
       <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="11">
         <v>46053.0</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="10">
         <v>1.0</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -1040,13 +1092,13 @@
       </c>
     </row>
     <row r="16">
-      <c r="I16" s="9">
+      <c r="I16" s="10">
         <v>2.0</v>
       </c>
-      <c r="J16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="J16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="8" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -1054,34 +1106,520 @@
       </c>
     </row>
     <row r="17">
-      <c r="I17" s="9">
+      <c r="I17" s="10">
         <v>3.0</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="I18" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="6">
+        <v>46055.0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="I18" s="9">
+      <c r="K20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="1">
         <v>4.0</v>
       </c>
-      <c r="J18" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="J22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="E19:E22"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: update Qa-roadmap with TC-06 test
</commit_message>
<xml_diff>
--- a/docs/QA_Roadmap_Natalia.xlsx
+++ b/docs/QA_Roadmap_Natalia.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>Validar el formato de precios ($)</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
   </si>
   <si>
     <r>
@@ -203,6 +200,35 @@
   <si>
     <t>Todos los precios contienen el símbolo "$" y el formato es numérico válido.</t>
   </si>
+  <si>
+    <t>TC-06</t>
+  </si>
+  <si>
+    <t>Validar nombres de productos contra listra maestra.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title, .inventory_item_price, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>.inventory_item_name</t>
+    </r>
+  </si>
+  <si>
+    <t>Extraer lista de nombres y verificar su exactitud</t>
+  </si>
+  <si>
+    <t>Todos los nombres de productos existen en orden y de forma correcta.</t>
+  </si>
 </sst>
 </file>
 
@@ -211,7 +237,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -226,12 +252,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -254,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -290,9 +310,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1144,10 +1161,10 @@
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>16</v>
@@ -1234,10 +1251,10 @@
         <v>3.0</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>20</v>
@@ -1270,10 +1287,10 @@
         <v>4.0</v>
       </c>
       <c r="J22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>20</v>
@@ -1295,18 +1312,42 @@
       <c r="AA22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="6">
+        <v>46056.0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -1328,14 +1369,21 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="I24" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -1357,14 +1405,21 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="I25" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -1386,14 +1441,21 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="I26" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
@@ -1614,11 +1676,12 @@
       <c r="AA33" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="E15:E18"/>
     <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E23:E26"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: update Readme, roadmap and and  control panel, with the content of session nine
</commit_message>
<xml_diff>
--- a/docs/QA_Roadmap_Natalia.xlsx
+++ b/docs/QA_Roadmap_Natalia.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -229,6 +229,64 @@
   <si>
     <t>Todos los nombres de productos existen en orden y de forma correcta.</t>
   </si>
+  <si>
+    <t>TC-07</t>
+  </si>
+  <si>
+    <t>Ordenamiento de precio (Low to High)</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title, .inventory_item_price, .inventory_item_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>.product_sort_container</t>
+    </r>
+  </si>
+  <si>
+    <t>Validar que el filtro de menor a mayor ordena numéricamente de forma ascendente.</t>
+  </si>
+  <si>
+    <t>Se obtienen los precios ordenados correctamente.</t>
+  </si>
+  <si>
+    <t>TC-08</t>
+  </si>
+  <si>
+    <t>Ordenamiento de precio (High to Low)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title, .inventory_item_price, .inventory_item_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>.product_sort_container</t>
+    </r>
+  </si>
+  <si>
+    <t>Validar que el filtro de mayor a menor ordena numéricamente de forma descendente.</t>
+  </si>
 </sst>
 </file>
 
@@ -237,7 +295,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -252,6 +310,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="'Google Sans Text'"/>
     </font>
   </fonts>
   <fills count="3">
@@ -303,12 +366,12 @@
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -528,22 +591,25 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="7.13"/>
-    <col customWidth="1" min="2" max="2" width="20.75"/>
+    <col customWidth="1" min="2" max="2" width="24.75"/>
     <col customWidth="1" min="3" max="3" width="9.38"/>
-    <col customWidth="1" min="4" max="4" width="8.63"/>
+    <col customWidth="1" min="4" max="4" width="11.13"/>
     <col customWidth="1" min="5" max="5" width="33.63"/>
     <col customWidth="1" min="6" max="6" width="14.38"/>
     <col customWidth="1" min="7" max="7" width="12.63"/>
     <col customWidth="1" min="8" max="8" width="11.13"/>
     <col customWidth="1" min="9" max="9" width="4.13"/>
-    <col customWidth="1" min="10" max="27" width="20.75"/>
+    <col customWidth="1" min="10" max="10" width="63.75"/>
+    <col customWidth="1" min="11" max="27" width="20.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -657,7 +723,6 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="9"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -694,7 +759,6 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="9"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -731,7 +795,6 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -768,7 +831,6 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="9"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="6"/>
@@ -981,7 +1043,7 @@
       <c r="I11" s="7">
         <v>1.0</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1063,7 +1125,7 @@
       <c r="J14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="9" t="s">
         <v>42</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1071,10 +1133,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1092,10 +1154,10 @@
       <c r="G15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>46053.0</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="9">
         <v>1.0</v>
       </c>
       <c r="J15" s="8" t="s">
@@ -1109,10 +1171,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="I16" s="10">
+      <c r="I16" s="9">
         <v>2.0</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="9" t="s">
         <v>46</v>
       </c>
       <c r="K16" s="8" t="s">
@@ -1123,13 +1185,13 @@
       </c>
     </row>
     <row r="17">
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>3.0</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="9" t="s">
         <v>48</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1137,13 +1199,13 @@
       </c>
     </row>
     <row r="18">
-      <c r="I18" s="10">
+      <c r="I18" s="9">
         <v>4.0</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="9" t="s">
         <v>50</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -1472,19 +1534,43 @@
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
     </row>
-    <row r="27">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+    <row r="27" ht="20.25" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="6">
+        <v>46057.0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -1501,19 +1587,26 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
     </row>
-    <row r="28">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+    <row r="28" ht="20.25" customHeight="1">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="I28" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -1530,19 +1623,26 @@
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
     </row>
-    <row r="29">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+    <row r="29" ht="20.25" customHeight="1">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="I29" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -1559,19 +1659,26 @@
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
     </row>
-    <row r="30">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+    <row r="30" ht="20.25" customHeight="1">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="I30" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
@@ -1589,18 +1696,42 @@
       <c r="AA30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="A31" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="6">
+        <v>46057.0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
@@ -1618,18 +1749,25 @@
       <c r="AA31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="I32" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
@@ -1651,14 +1789,21 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="I33" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
@@ -1675,13 +1820,142 @@
       <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
     </row>
+    <row r="34" ht="33.75" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+    </row>
+    <row r="45">
+      <c r="E45" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="E15:E18"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="E23:E26"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="E2:E6"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: update the roadmap with a TC-11 test
</commit_message>
<xml_diff>
--- a/docs/QA_Roadmap_Natalia.xlsx
+++ b/docs/QA_Roadmap_Natalia.xlsx
@@ -4,6 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Actualización de Test Case Auto" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Hoja 1" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Hoja 2" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -287,13 +289,135 @@
   <si>
     <t>Validar que el filtro de mayor a menor ordena numéricamente de forma descendente.</t>
   </si>
+  <si>
+    <t>TC-09</t>
+  </si>
+  <si>
+    <t>Ordenamiento de nombre de los productos (A to Z)</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title, .inventory_item_price, .inventory_item_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>.product_sort_container</t>
+    </r>
+  </si>
+  <si>
+    <t>Validar que el filtro (A to Z) ordena alfabéticamente de forma ascendente</t>
+  </si>
+  <si>
+    <t>Se obtienen los nombres ordenados correctamente</t>
+  </si>
+  <si>
+    <t>TC-10</t>
+  </si>
+  <si>
+    <t>Ordenamiento de nombre de los productos (Z to A)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title, .inventory_item_price, .inventory_item_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>.product_sort_container</t>
+    </r>
+  </si>
+  <si>
+    <t>Validar que el filtro (Z to A) ordena alfabéticamente de forma descendente</t>
+  </si>
+  <si>
+    <t>TC-11</t>
+  </si>
+  <si>
+    <t>Validar incremento del contador del carrito (Badge)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
+      </rPr>
+      <t>[data-test="login-button"], [data-test="username"], [data-test="password"], .inventory_list, .inventory_item, .title,</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> .shopping_cart_badge, .btn_inventory</t>
+    </r>
+  </si>
+  <si>
+    <t>❌ NO</t>
+  </si>
+  <si>
+    <t>PENDIENTE 🟡</t>
+  </si>
+  <si>
+    <t>Verificar estado inicial del carrito.</t>
+  </si>
+  <si>
+    <t>El badge (.shopping_cart_badge) no es visible o es 0.</t>
+  </si>
+  <si>
+    <t>Click en "Add to Cart" de un producto específico.</t>
+  </si>
+  <si>
+    <t>El botón cambia a "Remove".</t>
+  </si>
+  <si>
+    <t>Validar que el badge muestra el número "1".</t>
+  </si>
+  <si>
+    <t>El contador se incrementa correctamente.</t>
+  </si>
+  <si>
+    <t>PENDIENTE 🟡,</t>
+  </si>
+  <si>
+    <t>Estado 2</t>
+  </si>
+  <si>
+    <t>.shopping_cart_badge, .btn_inventory</t>
+  </si>
+  <si>
+    <t>Iniciar sesión con credenciales válidas.</t>
+  </si>
+  <si>
+    <t>Acceso exitoso al inventario.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="d/MM/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -312,12 +436,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="'Google Sans Text'"/>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +455,18 @@
         <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8F9"/>
+        <bgColor rgb="FFF6F8F9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -337,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -371,14 +508,148 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF535FC1"/>
+          <bgColor rgb="FF535FC1"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6F8F9"/>
+          <bgColor rgb="FFF6F8F9"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF535FC1"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF535FC1"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF535FC1"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF535FC1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1">
+    <tableStyle count="4" pivot="0" name="Hoja 2-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -386,8 +657,36 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A45:L49" displayName="Tabla_1" name="Tabla_1" id="1">
+  <tableColumns count="12">
+    <tableColumn name="ID" id="1"/>
+    <tableColumn name="Título del Test" id="2"/>
+    <tableColumn name="Prioridad" id="3"/>
+    <tableColumn name="Estado" id="4"/>
+    <tableColumn name="Selector" id="5"/>
+    <tableColumn name="Automatizado" id="6"/>
+    <tableColumn name="Resultado Final" id="7"/>
+    <tableColumn name="Fecha de Ejecución" id="8"/>
+    <tableColumn name="Paso" id="9"/>
+    <tableColumn name="Acción Técnica (Comentario en Código)" id="10"/>
+    <tableColumn name="Resultado Esperado" id="11"/>
+    <tableColumn name="Estado 2" id="12"/>
+  </tableColumns>
+  <tableStyleInfo name="Hoja 2-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,17 +898,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.13"/>
-    <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="1" max="1" width="5.63"/>
+    <col customWidth="1" min="2" max="2" width="39.13"/>
     <col customWidth="1" min="3" max="3" width="9.38"/>
-    <col customWidth="1" min="4" max="4" width="11.13"/>
-    <col customWidth="1" min="5" max="5" width="33.63"/>
+    <col customWidth="1" min="4" max="4" width="8.63"/>
+    <col customWidth="1" min="5" max="5" width="23.88"/>
     <col customWidth="1" min="6" max="6" width="14.38"/>
-    <col customWidth="1" min="7" max="7" width="12.63"/>
-    <col customWidth="1" min="8" max="8" width="11.13"/>
-    <col customWidth="1" min="9" max="9" width="4.13"/>
+    <col customWidth="1" min="7" max="7" width="13.13"/>
+    <col customWidth="1" min="8" max="8" width="15.63"/>
+    <col customWidth="1" min="9" max="9" width="4.75"/>
     <col customWidth="1" min="10" max="10" width="63.75"/>
-    <col customWidth="1" min="11" max="27" width="20.75"/>
+    <col customWidth="1" min="11" max="11" width="56.13"/>
+    <col customWidth="1" min="12" max="12" width="8.5"/>
+    <col customWidth="1" min="13" max="27" width="20.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1857,18 +2158,42 @@
       <c r="AA34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="A35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="6">
+        <v>46059.0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
@@ -1890,14 +2215,21 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+      <c r="I36" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
@@ -1919,14 +2251,21 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
+      <c r="I37" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
@@ -1943,20 +2282,500 @@
       <c r="Z37" s="3"/>
       <c r="AA37" s="3"/>
     </row>
+    <row r="38">
+      <c r="I38" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="L39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="L40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="6">
+        <v>46065.0</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="I42" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="I43" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="I44" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="45">
-      <c r="E45" s="11"/>
+      <c r="A45" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H45" s="14">
+        <v>46066.0</v>
+      </c>
+      <c r="I45" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="J46" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K46" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L46" s="22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="J47" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K47" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="L47" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="19"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="21">
+        <v>4.0</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K48" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="L48" s="22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="24"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="26">
+        <v>5.0</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="27"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="29">
+        <v>6.0</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K50" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="L50" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="24"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="27"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="E35:E39"/>
+    <mergeCell ref="E41:E44"/>
+    <mergeCell ref="E45:E50"/>
+    <mergeCell ref="E2:E6"/>
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="E15:E18"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="E27:E30"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="E2:E6"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="9.5"/>
+    <col customWidth="1" min="2" max="8" width="12.63"/>
+    <col customWidth="1" min="9" max="9" width="11.5"/>
+    <col customWidth="1" min="10" max="12" width="12.63"/>
+  </cols>
+  <sheetData>
+    <row r="45" ht="22.5" customHeight="1">
+      <c r="A45" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L45" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" ht="22.5" customHeight="1">
+      <c r="A46" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="H46" s="34">
+        <v>46066.0</v>
+      </c>
+      <c r="I46" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="J46" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="K46" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="L46" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" ht="22.5" customHeight="1">
+      <c r="A47" s="32"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="35">
+        <v>2.0</v>
+      </c>
+      <c r="J47" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K47" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="L47" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" ht="22.5" customHeight="1">
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="35">
+        <v>3.0</v>
+      </c>
+      <c r="J48" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="K48" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="L48" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" ht="22.5" customHeight="1">
+      <c r="A49" s="32"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="35">
+        <v>4.0</v>
+      </c>
+      <c r="J49" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K49" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="L49" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="H46:H49">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(H46))), AND(ISNUMBER(H46), LEFT(CELL("format", H46))="D"))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I46:I49">
+      <formula1>AND(ISNUMBER(I46),(NOT(OR(NOT(ISERROR(DATEVALUE(I46))), AND(ISNUMBER(I46), LEFT(CELL("format", I46))="D")))))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>